<commit_message>
reformulation finished. Cleaned up.
</commit_message>
<xml_diff>
--- a/input/similarity_c_c.xlsx
+++ b/input/similarity_c_c.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalUserData\User-data\feita1\Uni\PhD\Projects\French keyboard\Optimization\optimizing-the-french-keyboard\input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
   <si>
     <t>é</t>
   </si>
@@ -264,6 +259,27 @@
   </si>
   <si>
     <t>²</t>
+  </si>
+  <si>
+    <t>c'h</t>
+  </si>
+  <si>
+    <t>C'H</t>
+  </si>
+  <si>
+    <t>C'h</t>
+  </si>
+  <si>
+    <t>Ð</t>
+  </si>
+  <si>
+    <t>ð</t>
+  </si>
+  <si>
+    <t>Þ</t>
+  </si>
+  <si>
+    <t>þ</t>
   </si>
 </sst>
 </file>
@@ -625,7 +641,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -633,19 +649,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF81"/>
+  <dimension ref="A1:CJ88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="32" ySplit="19" topLeftCell="AG71" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG1" sqref="AG1"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A82:XFD88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="77" width="3.85546875" customWidth="1"/>
     <col min="78" max="81" width="3.42578125" customWidth="1"/>
+    <col min="82" max="82" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="85" max="88" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>56</v>
       </c>
@@ -886,11 +909,29 @@
       <c r="CC1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" s="3"/>
-      <c r="CE1" s="3"/>
-      <c r="CF1" s="3"/>
-    </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="CD1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -932,7 +973,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -972,7 +1013,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -1007,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1037,7 +1078,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
@@ -1068,7 +1109,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>66</v>
       </c>
@@ -1082,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
@@ -1109,7 +1150,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
@@ -1134,7 +1175,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1160,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1181,7 +1222,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1203,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1223,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1288,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -4820,7 +4861,7 @@
       <c r="CA80" s="7"/>
       <c r="CB80" s="7"/>
     </row>
-    <row r="81" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -4905,6 +4946,644 @@
       <c r="CB81" s="7"/>
       <c r="CC81" s="7"/>
     </row>
+    <row r="82" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="7"/>
+      <c r="K82" s="7"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="7"/>
+      <c r="N82" s="7"/>
+      <c r="O82" s="7"/>
+      <c r="P82" s="7"/>
+      <c r="Q82" s="7"/>
+      <c r="R82" s="7"/>
+      <c r="S82" s="7"/>
+      <c r="T82" s="7"/>
+      <c r="U82" s="7"/>
+      <c r="V82" s="7"/>
+      <c r="W82" s="7"/>
+      <c r="X82" s="7"/>
+      <c r="Y82" s="7"/>
+      <c r="Z82" s="7"/>
+      <c r="AA82" s="7"/>
+      <c r="AB82" s="7"/>
+      <c r="AC82" s="7"/>
+      <c r="AD82" s="7"/>
+      <c r="AE82" s="7"/>
+      <c r="AF82" s="7"/>
+      <c r="AG82" s="7"/>
+      <c r="AH82" s="7"/>
+      <c r="AI82" s="7"/>
+      <c r="AJ82" s="7"/>
+      <c r="AK82" s="7"/>
+      <c r="AL82" s="7"/>
+      <c r="AM82" s="7"/>
+      <c r="AN82" s="7"/>
+      <c r="AO82" s="7"/>
+      <c r="AP82" s="7"/>
+      <c r="AQ82" s="7"/>
+      <c r="AR82" s="7"/>
+      <c r="AS82" s="7"/>
+      <c r="AT82" s="7"/>
+      <c r="AU82" s="7"/>
+      <c r="AV82" s="7"/>
+      <c r="AW82" s="7"/>
+      <c r="AX82" s="7"/>
+      <c r="AY82" s="7"/>
+      <c r="AZ82" s="7"/>
+      <c r="BA82" s="7"/>
+      <c r="BB82" s="7"/>
+      <c r="BC82" s="7"/>
+      <c r="BD82" s="7"/>
+      <c r="BE82" s="7"/>
+      <c r="BF82" s="7"/>
+      <c r="BG82" s="7"/>
+      <c r="BH82" s="7"/>
+      <c r="BI82" s="7"/>
+      <c r="BJ82" s="7"/>
+      <c r="BK82" s="7"/>
+      <c r="BL82" s="7"/>
+      <c r="BM82" s="7"/>
+      <c r="BN82" s="7"/>
+      <c r="BO82" s="7"/>
+      <c r="BP82" s="7"/>
+      <c r="BQ82" s="7"/>
+      <c r="BR82" s="7"/>
+      <c r="BS82" s="7"/>
+      <c r="BT82" s="7"/>
+      <c r="BU82" s="7"/>
+      <c r="BV82" s="7"/>
+      <c r="BW82" s="7"/>
+      <c r="BX82" s="7"/>
+      <c r="BY82" s="7"/>
+      <c r="BZ82" s="7"/>
+      <c r="CA82" s="7"/>
+      <c r="CB82" s="7"/>
+      <c r="CC82" s="7"/>
+      <c r="CD82" s="7"/>
+      <c r="CE82">
+        <v>1</v>
+      </c>
+      <c r="CF82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="7"/>
+      <c r="P83" s="7"/>
+      <c r="Q83" s="7"/>
+      <c r="R83" s="7"/>
+      <c r="S83" s="7"/>
+      <c r="T83" s="7"/>
+      <c r="U83" s="7"/>
+      <c r="V83" s="7"/>
+      <c r="W83" s="7"/>
+      <c r="X83" s="7"/>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7"/>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7"/>
+      <c r="AC83" s="7"/>
+      <c r="AD83" s="7"/>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="7"/>
+      <c r="AG83" s="7"/>
+      <c r="AH83" s="7"/>
+      <c r="AI83" s="7"/>
+      <c r="AJ83" s="7"/>
+      <c r="AK83" s="7"/>
+      <c r="AL83" s="7"/>
+      <c r="AM83" s="7"/>
+      <c r="AN83" s="7"/>
+      <c r="AO83" s="7"/>
+      <c r="AP83" s="7"/>
+      <c r="AQ83" s="7"/>
+      <c r="AR83" s="7"/>
+      <c r="AS83" s="7"/>
+      <c r="AT83" s="7"/>
+      <c r="AU83" s="7"/>
+      <c r="AV83" s="7"/>
+      <c r="AW83" s="7"/>
+      <c r="AX83" s="7"/>
+      <c r="AY83" s="7"/>
+      <c r="AZ83" s="7"/>
+      <c r="BA83" s="7"/>
+      <c r="BB83" s="7"/>
+      <c r="BC83" s="7"/>
+      <c r="BD83" s="7"/>
+      <c r="BE83" s="7"/>
+      <c r="BF83" s="7"/>
+      <c r="BG83" s="7"/>
+      <c r="BH83" s="7"/>
+      <c r="BI83" s="7"/>
+      <c r="BJ83" s="7"/>
+      <c r="BK83" s="7"/>
+      <c r="BL83" s="7"/>
+      <c r="BM83" s="7"/>
+      <c r="BN83" s="7"/>
+      <c r="BO83" s="7"/>
+      <c r="BP83" s="7"/>
+      <c r="BQ83" s="7"/>
+      <c r="BR83" s="7"/>
+      <c r="BS83" s="7"/>
+      <c r="BT83" s="7"/>
+      <c r="BU83" s="7"/>
+      <c r="BV83" s="7"/>
+      <c r="BW83" s="7"/>
+      <c r="BX83" s="7"/>
+      <c r="BY83" s="7"/>
+      <c r="BZ83" s="7"/>
+      <c r="CA83" s="7"/>
+      <c r="CB83" s="7"/>
+      <c r="CC83" s="7"/>
+      <c r="CD83" s="7"/>
+      <c r="CE83" s="7"/>
+      <c r="CF83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="7"/>
+      <c r="K84" s="7"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="7"/>
+      <c r="N84" s="7"/>
+      <c r="O84" s="7"/>
+      <c r="P84" s="7"/>
+      <c r="Q84" s="7"/>
+      <c r="R84" s="7"/>
+      <c r="S84" s="7"/>
+      <c r="T84" s="7"/>
+      <c r="U84" s="7"/>
+      <c r="V84" s="7"/>
+      <c r="W84" s="7"/>
+      <c r="X84" s="7"/>
+      <c r="Y84" s="7"/>
+      <c r="Z84" s="7"/>
+      <c r="AA84" s="7"/>
+      <c r="AB84" s="7"/>
+      <c r="AC84" s="7"/>
+      <c r="AD84" s="7"/>
+      <c r="AE84" s="7"/>
+      <c r="AF84" s="7"/>
+      <c r="AG84" s="7"/>
+      <c r="AH84" s="7"/>
+      <c r="AI84" s="7"/>
+      <c r="AJ84" s="7"/>
+      <c r="AK84" s="7"/>
+      <c r="AL84" s="7"/>
+      <c r="AM84" s="7"/>
+      <c r="AN84" s="7"/>
+      <c r="AO84" s="7"/>
+      <c r="AP84" s="7"/>
+      <c r="AQ84" s="7"/>
+      <c r="AR84" s="7"/>
+      <c r="AS84" s="7"/>
+      <c r="AT84" s="7"/>
+      <c r="AU84" s="7"/>
+      <c r="AV84" s="7"/>
+      <c r="AW84" s="7"/>
+      <c r="AX84" s="7"/>
+      <c r="AY84" s="7"/>
+      <c r="AZ84" s="7"/>
+      <c r="BA84" s="7"/>
+      <c r="BB84" s="7"/>
+      <c r="BC84" s="7"/>
+      <c r="BD84" s="7"/>
+      <c r="BE84" s="7"/>
+      <c r="BF84" s="7"/>
+      <c r="BG84" s="7"/>
+      <c r="BH84" s="7"/>
+      <c r="BI84" s="7"/>
+      <c r="BJ84" s="7"/>
+      <c r="BK84" s="7"/>
+      <c r="BL84" s="7"/>
+      <c r="BM84" s="7"/>
+      <c r="BN84" s="7"/>
+      <c r="BO84" s="7"/>
+      <c r="BP84" s="7"/>
+      <c r="BQ84" s="7"/>
+      <c r="BR84" s="7"/>
+      <c r="BS84" s="7"/>
+      <c r="BT84" s="7"/>
+      <c r="BU84" s="7"/>
+      <c r="BV84" s="7"/>
+      <c r="BW84" s="7"/>
+      <c r="BX84" s="7"/>
+      <c r="BY84" s="7"/>
+      <c r="BZ84" s="7"/>
+      <c r="CA84" s="7"/>
+      <c r="CB84" s="7"/>
+      <c r="CC84" s="7"/>
+      <c r="CD84" s="7"/>
+      <c r="CE84" s="7"/>
+      <c r="CF84" s="7"/>
+    </row>
+    <row r="85" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="7"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="7"/>
+      <c r="P85" s="7"/>
+      <c r="Q85" s="7"/>
+      <c r="R85" s="7"/>
+      <c r="S85" s="7"/>
+      <c r="T85" s="7"/>
+      <c r="U85" s="7"/>
+      <c r="V85" s="7"/>
+      <c r="W85" s="7"/>
+      <c r="X85" s="7"/>
+      <c r="Y85" s="7"/>
+      <c r="Z85" s="7"/>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7"/>
+      <c r="AC85" s="7"/>
+      <c r="AD85" s="7"/>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
+      <c r="AG85" s="7"/>
+      <c r="AH85" s="7"/>
+      <c r="AI85" s="7"/>
+      <c r="AJ85" s="7"/>
+      <c r="AK85" s="7"/>
+      <c r="AL85" s="7"/>
+      <c r="AM85" s="7"/>
+      <c r="AN85" s="7"/>
+      <c r="AO85" s="7"/>
+      <c r="AP85" s="7"/>
+      <c r="AQ85" s="7"/>
+      <c r="AR85" s="7"/>
+      <c r="AS85" s="7"/>
+      <c r="AT85" s="7"/>
+      <c r="AU85" s="7"/>
+      <c r="AV85" s="7"/>
+      <c r="AW85" s="7"/>
+      <c r="AX85" s="7"/>
+      <c r="AY85" s="7"/>
+      <c r="AZ85" s="7"/>
+      <c r="BA85" s="7"/>
+      <c r="BB85" s="7"/>
+      <c r="BC85" s="7"/>
+      <c r="BD85" s="7"/>
+      <c r="BE85" s="7"/>
+      <c r="BF85" s="7"/>
+      <c r="BG85" s="7"/>
+      <c r="BH85" s="7"/>
+      <c r="BI85" s="7"/>
+      <c r="BJ85" s="7"/>
+      <c r="BK85" s="7"/>
+      <c r="BL85" s="7"/>
+      <c r="BM85" s="7"/>
+      <c r="BN85" s="7"/>
+      <c r="BO85" s="7"/>
+      <c r="BP85" s="7"/>
+      <c r="BQ85" s="7"/>
+      <c r="BR85" s="7"/>
+      <c r="BS85" s="7"/>
+      <c r="BT85" s="7"/>
+      <c r="BU85" s="7"/>
+      <c r="BV85" s="7"/>
+      <c r="BW85" s="7"/>
+      <c r="BX85" s="7"/>
+      <c r="BY85" s="7"/>
+      <c r="BZ85" s="7"/>
+      <c r="CA85" s="7"/>
+      <c r="CB85" s="7"/>
+      <c r="CC85" s="7"/>
+      <c r="CD85" s="7"/>
+      <c r="CE85" s="7"/>
+      <c r="CF85" s="7"/>
+      <c r="CG85" s="7"/>
+      <c r="CH85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="7"/>
+      <c r="N86" s="7"/>
+      <c r="O86" s="7"/>
+      <c r="P86" s="7"/>
+      <c r="Q86" s="7"/>
+      <c r="R86" s="7"/>
+      <c r="S86" s="7"/>
+      <c r="T86" s="7"/>
+      <c r="U86" s="7"/>
+      <c r="V86" s="7"/>
+      <c r="W86" s="7"/>
+      <c r="X86" s="7"/>
+      <c r="Y86" s="7"/>
+      <c r="Z86" s="7"/>
+      <c r="AA86" s="7"/>
+      <c r="AB86" s="7"/>
+      <c r="AC86" s="7"/>
+      <c r="AD86" s="7"/>
+      <c r="AE86" s="7"/>
+      <c r="AF86" s="7"/>
+      <c r="AG86" s="7"/>
+      <c r="AH86" s="7"/>
+      <c r="AI86" s="7"/>
+      <c r="AJ86" s="7"/>
+      <c r="AK86" s="7"/>
+      <c r="AL86" s="7"/>
+      <c r="AM86" s="7"/>
+      <c r="AN86" s="7"/>
+      <c r="AO86" s="7"/>
+      <c r="AP86" s="7"/>
+      <c r="AQ86" s="7"/>
+      <c r="AR86" s="7"/>
+      <c r="AS86" s="7"/>
+      <c r="AT86" s="7"/>
+      <c r="AU86" s="7"/>
+      <c r="AV86" s="7"/>
+      <c r="AW86" s="7"/>
+      <c r="AX86" s="7"/>
+      <c r="AY86" s="7"/>
+      <c r="AZ86" s="7"/>
+      <c r="BA86" s="7"/>
+      <c r="BB86" s="7"/>
+      <c r="BC86" s="7"/>
+      <c r="BD86" s="7"/>
+      <c r="BE86" s="7"/>
+      <c r="BF86" s="7"/>
+      <c r="BG86" s="7"/>
+      <c r="BH86" s="7"/>
+      <c r="BI86" s="7"/>
+      <c r="BJ86" s="7"/>
+      <c r="BK86" s="7"/>
+      <c r="BL86" s="7"/>
+      <c r="BM86" s="7"/>
+      <c r="BN86" s="7"/>
+      <c r="BO86" s="7"/>
+      <c r="BP86" s="7"/>
+      <c r="BQ86" s="7"/>
+      <c r="BR86" s="7"/>
+      <c r="BS86" s="7"/>
+      <c r="BT86" s="7"/>
+      <c r="BU86" s="7"/>
+      <c r="BV86" s="7"/>
+      <c r="BW86" s="7"/>
+      <c r="BX86" s="7"/>
+      <c r="BY86" s="7"/>
+      <c r="BZ86" s="7"/>
+      <c r="CA86" s="7"/>
+      <c r="CB86" s="7"/>
+      <c r="CC86" s="7"/>
+      <c r="CD86" s="7"/>
+      <c r="CE86" s="7"/>
+      <c r="CF86" s="7"/>
+      <c r="CG86" s="7"/>
+      <c r="CH86" s="7"/>
+    </row>
+    <row r="87" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="7"/>
+      <c r="N87" s="7"/>
+      <c r="O87" s="7"/>
+      <c r="P87" s="7"/>
+      <c r="Q87" s="7"/>
+      <c r="R87" s="7"/>
+      <c r="S87" s="7"/>
+      <c r="T87" s="7"/>
+      <c r="U87" s="7"/>
+      <c r="V87" s="7"/>
+      <c r="W87" s="7"/>
+      <c r="X87" s="7"/>
+      <c r="Y87" s="7"/>
+      <c r="Z87" s="7"/>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7"/>
+      <c r="AC87" s="7"/>
+      <c r="AD87" s="7"/>
+      <c r="AE87" s="7"/>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="7"/>
+      <c r="AH87" s="7"/>
+      <c r="AI87" s="7"/>
+      <c r="AJ87" s="7"/>
+      <c r="AK87" s="7"/>
+      <c r="AL87" s="7"/>
+      <c r="AM87" s="7"/>
+      <c r="AN87" s="7"/>
+      <c r="AO87" s="7"/>
+      <c r="AP87" s="7"/>
+      <c r="AQ87" s="7"/>
+      <c r="AR87" s="7"/>
+      <c r="AS87" s="7"/>
+      <c r="AT87" s="7"/>
+      <c r="AU87" s="7"/>
+      <c r="AV87" s="7"/>
+      <c r="AW87" s="7"/>
+      <c r="AX87" s="7"/>
+      <c r="AY87" s="7"/>
+      <c r="AZ87" s="7"/>
+      <c r="BA87" s="7"/>
+      <c r="BB87" s="7"/>
+      <c r="BC87" s="7"/>
+      <c r="BD87" s="7"/>
+      <c r="BE87" s="7"/>
+      <c r="BF87" s="7"/>
+      <c r="BG87" s="7"/>
+      <c r="BH87" s="7"/>
+      <c r="BI87" s="7"/>
+      <c r="BJ87" s="7"/>
+      <c r="BK87" s="7"/>
+      <c r="BL87" s="7"/>
+      <c r="BM87" s="7"/>
+      <c r="BN87" s="7"/>
+      <c r="BO87" s="7"/>
+      <c r="BP87" s="7"/>
+      <c r="BQ87" s="7"/>
+      <c r="BR87" s="7"/>
+      <c r="BS87" s="7"/>
+      <c r="BT87" s="7"/>
+      <c r="BU87" s="7"/>
+      <c r="BV87" s="7"/>
+      <c r="BW87" s="7"/>
+      <c r="BX87" s="7"/>
+      <c r="BY87" s="7"/>
+      <c r="BZ87" s="7"/>
+      <c r="CA87" s="7"/>
+      <c r="CB87" s="7"/>
+      <c r="CC87" s="7"/>
+      <c r="CD87" s="7"/>
+      <c r="CE87" s="7"/>
+      <c r="CF87" s="7"/>
+      <c r="CG87" s="7"/>
+      <c r="CH87" s="7"/>
+      <c r="CI87" s="7"/>
+      <c r="CJ87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="7"/>
+      <c r="K88" s="7"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="7"/>
+      <c r="N88" s="7"/>
+      <c r="O88" s="7"/>
+      <c r="P88" s="7"/>
+      <c r="Q88" s="7"/>
+      <c r="R88" s="7"/>
+      <c r="S88" s="7"/>
+      <c r="T88" s="7"/>
+      <c r="U88" s="7"/>
+      <c r="V88" s="7"/>
+      <c r="W88" s="7"/>
+      <c r="X88" s="7"/>
+      <c r="Y88" s="7"/>
+      <c r="Z88" s="7"/>
+      <c r="AA88" s="7"/>
+      <c r="AB88" s="7"/>
+      <c r="AC88" s="7"/>
+      <c r="AD88" s="7"/>
+      <c r="AE88" s="7"/>
+      <c r="AF88" s="7"/>
+      <c r="AG88" s="7"/>
+      <c r="AH88" s="7"/>
+      <c r="AI88" s="7"/>
+      <c r="AJ88" s="7"/>
+      <c r="AK88" s="7"/>
+      <c r="AL88" s="7"/>
+      <c r="AM88" s="7"/>
+      <c r="AN88" s="7"/>
+      <c r="AO88" s="7"/>
+      <c r="AP88" s="7"/>
+      <c r="AQ88" s="7"/>
+      <c r="AR88" s="7"/>
+      <c r="AS88" s="7"/>
+      <c r="AT88" s="7"/>
+      <c r="AU88" s="7"/>
+      <c r="AV88" s="7"/>
+      <c r="AW88" s="7"/>
+      <c r="AX88" s="7"/>
+      <c r="AY88" s="7"/>
+      <c r="AZ88" s="7"/>
+      <c r="BA88" s="7"/>
+      <c r="BB88" s="7"/>
+      <c r="BC88" s="7"/>
+      <c r="BD88" s="7"/>
+      <c r="BE88" s="7"/>
+      <c r="BF88" s="7"/>
+      <c r="BG88" s="7"/>
+      <c r="BH88" s="7"/>
+      <c r="BI88" s="7"/>
+      <c r="BJ88" s="7"/>
+      <c r="BK88" s="7"/>
+      <c r="BL88" s="7"/>
+      <c r="BM88" s="7"/>
+      <c r="BN88" s="7"/>
+      <c r="BO88" s="7"/>
+      <c r="BP88" s="7"/>
+      <c r="BQ88" s="7"/>
+      <c r="BR88" s="7"/>
+      <c r="BS88" s="7"/>
+      <c r="BT88" s="7"/>
+      <c r="BU88" s="7"/>
+      <c r="BV88" s="7"/>
+      <c r="BW88" s="7"/>
+      <c r="BX88" s="7"/>
+      <c r="BY88" s="7"/>
+      <c r="BZ88" s="7"/>
+      <c r="CA88" s="7"/>
+      <c r="CB88" s="7"/>
+      <c r="CC88" s="7"/>
+      <c r="CD88" s="7"/>
+      <c r="CE88" s="7"/>
+      <c r="CF88" s="7"/>
+      <c r="CG88" s="7"/>
+      <c r="CH88" s="7"/>
+      <c r="CI88" s="7"/>
+      <c r="CJ88" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>